<commit_message>
Version 1.4 in progress
The mail functionality as well as the side bar were unified with 2 working charts
</commit_message>
<xml_diff>
--- a/build/classes/files/asociados.xlsx
+++ b/build/classes/files/asociados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TEC\II SEMESTRE\Progra Orientada a Objetos\TAREAS PROGRAMADAS\TAREA 1\PROYECTO JAVA\Proyecto-1-POO\src\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\TEC\II semestre 2021\POO\proyecto1\Proyecto-1-POO\src\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4D26F0-4AD6-44C1-B76F-B5A749D0F0FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1FA544-C209-41C6-8FF4-9A89992944DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4845" yWindow="3630" windowWidth="19020" windowHeight="8910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6465" yWindow="3825" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Nombre</t>
   </si>
@@ -59,6 +59,21 @@
   </si>
   <si>
     <t>erisolfer@gmail.com</t>
+  </si>
+  <si>
+    <t>cesarjjxd@gmail.com</t>
+  </si>
+  <si>
+    <t>8529-6827</t>
+  </si>
+  <si>
+    <t>8598-6048</t>
+  </si>
+  <si>
+    <t>San José,Heredia,Cartago</t>
+  </si>
+  <si>
+    <t>San José,Heredia,Cartago,Alajuela,Puntarenas</t>
   </si>
 </sst>
 </file>
@@ -109,7 +124,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -126,7 +141,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -425,15 +440,15 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" customWidth="1"/>
     <col min="3" max="3" width="32" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="48.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -461,7 +476,7 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -472,22 +487,24 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -509,8 +526,9 @@
     <hyperlink ref="B2" r:id="rId1" xr:uid="{4261CDFF-C8DA-49EF-B270-A563B590788F}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{B49269CD-C585-47FA-91E8-45D2CD1D9115}"/>
     <hyperlink ref="B5" r:id="rId3" xr:uid="{BF082ADF-5FC2-492B-B3A4-3F3AFCF25723}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{6B4B889A-C166-40C8-8E93-FB6D377FEF87}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>